<commit_message>
sprint 105 Actual output and result
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33898339-57B2-47CD-A592-4601ACFCC3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF8B72D-866C-42E0-AA80-425ACF39EAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1525,7 +1525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sprint 107 manual testcases
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3324BD31-0A12-4249-A266-CCBD787A860E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6AF80A-C3D1-44E2-91ED-847D21126A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
   <si>
     <t>SL. No</t>
   </si>
@@ -988,6 +988,12 @@
     <t>When recording an adjustment, if "Transfer out" is selected as the reason, a checkbox ("Transfer to") with a dropdown to select the destination outlet is displayed below.</t>
   </si>
   <si>
+    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment-&gt;                Transfer out(new)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment-&gt;                Transfer In(new)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">By clicking Record adjustment ,it shows pop up screen </t>
     </r>
@@ -1000,149 +1006,143 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>"Item name dropdown, Inventory list, UOM, Quantity, Reason, From checkbox(new),Notes and Save"</t>
+    </r>
+  </si>
+  <si>
+    <t>In From checkout select location dropdown</t>
+  </si>
+  <si>
+    <t>Outlets -&gt; SKU-&gt;Consumption report</t>
+  </si>
+  <si>
+    <t>Outlets -&gt; SKU-&gt;Consumption report(New)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To display these columns, user has to select </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Show/hide columns"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and select the columns to be displayed or hidden.                                         *Below the Report "Show/hide colums " Once click the Show/hide colums it shows list of consumption report and Save</t>
+    </r>
+  </si>
+  <si>
+    <t>It gets displayed the Only selected columns the Show/hide colums</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">it shows pop up page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Outlet dropdown, Inventory list dropdown, Count date and start stock count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Click on the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> UOM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,it shows "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Activity and Settings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" page and once click on the Date </t>
+    </r>
+  </si>
+  <si>
+    <t>It gets displayed successfully</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On the top SKU name below it shows </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Inventory list: . Supplier: Outlet name"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note : In 2 outlets should have the same SKU then we can adjust the Transfer out/Transfer in, By clicking Record adjustment ,it shows pop up screen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>"Item name dropdown, Inventory list, UOM, Quantity, Reason, To checkbox(new),Notes and Save"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment-&gt;                Transfer out(new)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment-&gt;                Transfer In(new)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">By clicking Record adjustment ,it shows pop up screen </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Item name dropdown, Inventory list, UOM, Quantity, Reason, From checkbox(new),Notes and Save"</t>
-    </r>
-  </si>
-  <si>
-    <t>In From checkout select location dropdown</t>
-  </si>
-  <si>
-    <t>Outlets -&gt; SKU-&gt;Consumption report</t>
-  </si>
-  <si>
-    <t>Outlets -&gt; SKU-&gt;Consumption report(New)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">To display these columns, user has to select </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Show/hide columns"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and select the columns to be displayed or hidden.                                         *Below the Report "Show/hide colums " Once click the Show/hide colums it shows list of consumption report and Save</t>
-    </r>
-  </si>
-  <si>
-    <t>It gets displayed the Only selected columns the Show/hide colums</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">it shows pop up page </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Outlet dropdown, Inventory list dropdown, Count date and start stock count</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Click on the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> UOM </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,it shows "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Activity and Settings</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" page and once click on the Date </t>
-    </r>
-  </si>
-  <si>
-    <t>It gets displayed successfully</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">On the top SKU name below it shows </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Inventory list: . Supplier: Outlet name"</t>
     </r>
   </si>
 </sst>
@@ -1187,8 +1187,7 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF172B4D"/>
+      <sz val="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -1576,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1673,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>82</v>
@@ -1697,7 +1696,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>80</v>
@@ -1720,7 +1719,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>81</v>
@@ -1743,13 +1742,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>11</v>
@@ -2091,7 +2090,7 @@
         <v>34</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>35</v>
@@ -2146,7 +2145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2157,10 +2156,10 @@
         <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>50</v>
@@ -2180,17 +2179,19 @@
         <v>13</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2319,7 +2320,7 @@
         <v>79</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>77</v>
@@ -2342,10 +2343,10 @@
         <v>79</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Stock count can be saved with empty
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48652ACA-34CA-475B-B815-C9BD9A047B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8295983A-8076-4FBB-A64E-C0EBA4131A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="97">
   <si>
     <t>SL. No</t>
   </si>
@@ -1086,6 +1086,12 @@
   </si>
   <si>
     <t>If user has not entered the quantity for all items, the confirmation step will ask whether to "Save with blank fields automatically filled" in with '0'</t>
+  </si>
+  <si>
+    <t>It gets displayed the as expected</t>
+  </si>
+  <si>
+    <t>It gets displayed the pop up as expected</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,8 +2064,12 @@
       <c r="E23" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="10"/>
+      <c r="F23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2077,8 +2087,12 @@
       <c r="E24" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
+      <c r="F24" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2122,7 +2136,9 @@
       <c r="F26" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="10"/>
+      <c r="G26" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -2258,8 +2274,11 @@
       <c r="F32" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2277,6 +2296,9 @@
       </c>
       <c r="F33" s="9" t="s">
         <v>83</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stock count as draft
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B35B1D6-86EF-451E-AF61-27572ED55EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B55A52-3860-463E-B000-A0FDB8777284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="100">
   <si>
     <t>SL. No</t>
   </si>
@@ -936,6 +936,267 @@
     <t>In From checkout select location dropdown</t>
   </si>
   <si>
+    <t>Outlets -&gt; SKU-&gt;New stock count(new)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment-&gt;                Transfer out</t>
+  </si>
+  <si>
+    <t>Outlets -&gt; SKU &gt;Consumption report</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.It will shows Adjustment record page like </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Outlet, Reason, Item name, Inventory list, UOM, Quantity, Notes and Save" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                 2. Click Save ,Toaster message is Inventory added                               </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Once click the Save as draft, dialog box will appear Previously saved draft available and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Use draft and Start new stock count" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>It gets displayed the as expected</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There is a new </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select most recent date range"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button next to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Date'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field. When clicked, it automatically fills in the start and end dates with the two most recent selectable dates from the calendar picker.</t>
+    </r>
+  </si>
+  <si>
+    <t>It gets displayed Select most recent date range once we select the Inventory list</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It displayed the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Report and stock count"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                          1.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Report </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: it displayed SKU, UOM, Prev.qty, Purchased, Adjustments, End qty, Consumed(qty), Consumed</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">($)             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>below this</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Eye icon Show/hide columns                                     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Stock count </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Date, List, Created by, Est. value</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Select Outlet and Inventory and click</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Start stock count</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ,it goes to New </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stock count page</t>
+    </r>
+  </si>
+  <si>
+    <t>It dispalyed New stock count screen, SKU name search box, Name, Supplier, UOM, Last count, Counted, Qty,Cancel and Done</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">it shows pop up page </t>
     </r>
@@ -948,273 +1209,54 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Outlet dropdown, Inventory list dropdown, Count date(By default select the todays date) and start stock count</t>
-    </r>
-  </si>
-  <si>
-    <t>Outlets -&gt; SKU-&gt;New stock count(new)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Outlets-&gt;SKU-&gt; Record adjustment-&gt;                Transfer out</t>
-  </si>
-  <si>
-    <t>Outlets -&gt; SKU &gt;Consumption report</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.It will shows Adjustment record page like </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Outlet, Reason, Item name, Inventory list, UOM, Quantity, Notes and Save" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                 2. Click Save ,Toaster message is Inventory added                               </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Once click the Save as draft, dialog box will appear Previously saved draft available and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Use draft and Start new stock count" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>It gets displayed the as expected</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">There is a new </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select most recent date range"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> button next to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Date'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field. When clicked, it automatically fills in the start and end dates with the two most recent selectable dates from the calendar picker.</t>
-    </r>
-  </si>
-  <si>
-    <t>It gets displayed Select most recent date range once we select the Inventory list</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">It displayed the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Report and stock count"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                          1.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Report </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: it displayed SKU, UOM, Prev.qty, Purchased, Adjustments, End qty, Consumed(qty), Consumed</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">($)             </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>below this</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Eye icon Show/hide columns                                     </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Stock count </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Date, List, Created by, Est. value</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Select Outlet and Inventory and click</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Start stock count</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ,it goes to New </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>stock count page</t>
-    </r>
-  </si>
-  <si>
-    <t>It dispalyed New stock count screen, SKU name search box, Name, Supplier, UOM, Last count, Counted, Qty,Cancel and Done</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.User can still save the stock count and Auto-fill with last count data with '0' if wanted.                                                                                                       2.Click the </t>
+      <t>Outlet dropdown, Inventory list dropdown and start stock count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.Next to Cancel ,user can click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Save as Draft'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button at the buttom of the screen                                                                                                                                 If user has not entered the quantity for all items, the confirmation step will ask whether to "Save with blank fields automatically filled" in with '0'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It displayed toastr </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stock count Saved as draft successfully</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On top below New stock count 'Count date calendar picker                               1.User can still save the stock count and Auto-fill with last count data with '0' if wanted.                                                                                                       2.Click the </t>
     </r>
     <r>
       <rPr>
@@ -1235,39 +1277,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">,it shows Are you sure? pop up page </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cancel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Yes,fill in blank fields &amp; Save                                                                    </t>
+      <t xml:space="preserve">,it shows </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Update stock count</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">' pop up page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Save stock count                                                                 </t>
     </r>
     <r>
       <rPr>
@@ -1290,9 +1332,6 @@
       </rPr>
       <t xml:space="preserve">        </t>
     </r>
-  </si>
-  <si>
-    <t>3.Next to Cancel ,user can click 'Save as Draft' button at the buttom of the screen                                                                                                                                 If user has not entered the quantity for all items, the confirmation step will ask whether to "Save with blank fields automatically filled" in with '0'</t>
   </si>
 </sst>
 </file>
@@ -1715,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,7 +1852,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>78</v>
@@ -1836,7 +1875,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>76</v>
@@ -1859,13 +1898,13 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>11</v>
@@ -1885,10 +1924,10 @@
         <v>63</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>11</v>
@@ -2138,7 +2177,7 @@
         <v>61</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>41</v>
@@ -2230,7 +2269,7 @@
         <v>34</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>35</v>
@@ -2253,16 +2292,16 @@
         <v>34</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="G23" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2273,13 +2312,13 @@
         <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>11</v>
@@ -2296,13 +2335,17 @@
         <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2315,7 +2358,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Improvements of Stock count
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Outlets-SKU testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADA2BF9-B992-4AA7-A679-8ABEF01F4671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9625D3C8-D50D-4F21-BC4A-B6B7F990FF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="119">
   <si>
     <t>SL. No</t>
   </si>
@@ -1137,9 +1137,6 @@
     <t>3.Next to Cancel ,user can click 'Save as Draft' button at the buttom of the screen                                                                                                                                 If user has not entered the quantity for all items, the confirmation step will ask whether to "Save with blank fields automatically filled" in with '0'</t>
   </si>
   <si>
-    <t xml:space="preserve">The inventory UOM next to each item’s quantity field will be hyperlinked (in blue) and there is a down chevron symbol next to it. The label and the chevron are clickable as a button.                                     *Once click the UOM,it shows list and qty field next to each UOM and click Save </t>
-  </si>
-  <si>
     <t>Once edit UOM and qty and Save it gets dispalyed the updated result</t>
   </si>
   <si>
@@ -1608,6 +1605,10 @@
       </rPr>
       <t xml:space="preserve">                        </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory UOM next to each item’s quantity field will be hyperlinked (in blue) and there is a down chevron symbol next to it. The label and the chevron are clickable as a button.                                    
+ *Once click the UOM,it shows list and qty field next to each UOM and click Save </t>
   </si>
 </sst>
 </file>
@@ -2033,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2088,7 +2089,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>15</v>
@@ -2223,13 +2224,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>11</v>
@@ -2246,13 +2247,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>11</v>
@@ -2430,10 +2431,10 @@
         <v>9</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>15</v>
@@ -2450,7 +2451,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>31</v>
@@ -2502,7 +2503,7 @@
         <v>28</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>15</v>
@@ -2591,10 +2592,10 @@
         <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="6"/>
@@ -2728,10 +2729,10 @@
         <v>77</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>11</v>
@@ -2748,7 +2749,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>73</v>
@@ -2771,7 +2772,7 @@
         <v>13</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>74</v>
@@ -2794,7 +2795,7 @@
         <v>13</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>72</v>
@@ -2820,7 +2821,7 @@
         <v>47</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>50</v>
@@ -2846,7 +2847,7 @@
         <v>53</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>11</v>
@@ -2869,7 +2870,7 @@
         <v>55</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>11</v>
@@ -2909,15 +2910,17 @@
         <v>13</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="F38" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G38" s="6"/>
+        <v>99</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="119" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39">
@@ -2933,12 +2936,14 @@
         <v>66</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="6"/>
+        <v>116</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40">
@@ -2951,13 +2956,13 @@
         <v>13</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>11</v>
@@ -2974,13 +2979,13 @@
         <v>13</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>11</v>

</xml_diff>